<commit_message>
use old excel conv for xml
</commit_message>
<xml_diff>
--- a/server/php/sample.xlsx
+++ b/server/php/sample.xlsx
@@ -5,20 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -109,47 +113,21 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.73"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>